<commit_message>
i dont remember what i did here
</commit_message>
<xml_diff>
--- a/receipts.xlsx
+++ b/receipts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,6 +574,23 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11.12</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Found</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added load excel file functionality
</commit_message>
<xml_diff>
--- a/receipts.xlsx
+++ b/receipts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,63 +441,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 20.0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
+          <t>11/13/17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 20.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
+          <t>04/07/2017</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>11/13/17</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> d</t>
+          <t xml:space="preserve"> 23.19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Not Found</t>
+          <t xml:space="preserve"> Walmart</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> d</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -509,134 +489,49 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 11/13/17</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 23.19</t>
+          <t xml:space="preserve"> N</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Walmart</t>
+          <t xml:space="preserve"> Not Found</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04/07/2017</t>
+          <t xml:space="preserve"> 11/13/17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 29.01</t>
+          <t xml:space="preserve"> 23.19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Not Found</t>
+          <t xml:space="preserve"> Walmart</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N</t>
+          <t xml:space="preserve"> 04/07/2017</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N</t>
+          <t xml:space="preserve"> 29.01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 11.12</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 11/13/17</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 23.19</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Walmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04/07/2017</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 29.01</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve"> Not Found</t>
         </is>

</xml_diff>

<commit_message>
Added proper submit functionality, and added an unused new file function
</commit_message>
<xml_diff>
--- a/receipts.xlsx
+++ b/receipts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,105 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>11/13/17</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>04/07/2017</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>11/13/17</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 23.19</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Walmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 11/13/17</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 23.19</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Walmart</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04/07/2017</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 29.01</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Not Found</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>